<commit_message>
Moved Oldreplacercode.txt to the workshop folder Move FLAT DISAMBIGUATOR to workshop folder These files dont belong in the pk3.
</commit_message>
<xml_diff>
--- a/workshop/FLAT DISAMBIGUATOR.xlsx
+++ b/workshop/FLAT DISAMBIGUATOR.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="546">
   <si>
     <t>Name</t>
   </si>
@@ -906,6 +906,9 @@
     <t>ALWAYS</t>
   </si>
   <si>
+    <t>C:\Users\TwoIsOne\Desktop\5.22.19\WORKSPACE5\pk3\Flats\2\</t>
+  </si>
+  <si>
     <t>BRIKGTH1</t>
   </si>
   <si>
@@ -1551,6 +1554,24 @@
     <t>Paycloseattentiontotheprocessanddocumentittotryandmakeitmakesense.</t>
   </si>
   <si>
+    <t>usethenewcolumnstoshownewiterations</t>
+  </si>
+  <si>
+    <t>nexttimesortwadsbydatethistimeleadingbackto5.25.19</t>
+  </si>
+  <si>
+    <t>Thencutpastethembackintotheflatsfolderoverridingtheoriginalflats,withoutdeselectingdeletetheselectedflats.</t>
+  </si>
+  <si>
+    <t>Deletingtheoldflatsisrightbecausethetexureswillmakethemup…right???Yesthisisrightdeletetheoldflats</t>
+  </si>
+  <si>
+    <t>Todeletetheoriginalscopyallflatsintotexturefolder,cutthembacktotheflatsfolder,removethesfromthefolderandputtheminasubfolder.</t>
+  </si>
+  <si>
+    <t>Usethebulkutilitytotakeofftheanddon’tforgetthespace</t>
+  </si>
+  <si>
     <t>ADEL_F10</t>
   </si>
   <si>
@@ -1564,6 +1585,15 @@
   </si>
   <si>
     <t>RED</t>
+  </si>
+  <si>
+    <t>To properly do a texture flat disambiguation you need the original doom2 textures in</t>
+  </si>
+  <si>
+    <t>I made some sort of mistake here. These flats are most likely missing.</t>
+  </si>
+  <si>
+    <t>End of missing flats</t>
   </si>
   <si>
     <t>FD170</t>
@@ -2032,136 +2062,91 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B193" sqref="B193"/>
+    <sheetView tabSelected="1" topLeftCell="E185" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="H189" sqref="H189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" customWidth="1"/>
-    <col min="5" max="5" width="128.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="3" max="6" width="11.5703125" customWidth="1"/>
     <col min="12" max="12" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
       </c>
       <c r="L1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
       <c r="L2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G3" t="s">
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
         <v>9</v>
       </c>
       <c r="G4" t="s">
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
       <c r="L5" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>160</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s">
         <v>11</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
       </c>
       <c r="L6" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>161</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s">
         <v>12</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
       </c>
       <c r="L7" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>162</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
         <v>13</v>
       </c>
       <c r="G8" t="s">
@@ -2173,458 +2158,365 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>163</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" t="s">
         <v>14</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
       </c>
       <c r="L9" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>164</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="G10" t="s">
         <v>2</v>
       </c>
       <c r="L10" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>165</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
       <c r="L11" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>166</v>
-      </c>
-      <c r="B12" t="s">
-        <v>27</v>
+        <v>523</v>
       </c>
       <c r="L12" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>167</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
       <c r="H13" t="s">
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>168</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>169</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
       <c r="H15" t="s">
         <v>1</v>
       </c>
       <c r="L15" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>170</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>296</v>
       </c>
       <c r="H16" t="s">
         <v>15</v>
       </c>
       <c r="L16" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>171</v>
-      </c>
+        <v>370</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" t="s">
         <v>155</v>
       </c>
       <c r="H17" t="s">
         <v>16</v>
       </c>
       <c r="L17" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>172</v>
-      </c>
+        <v>371</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" t="s">
         <v>156</v>
       </c>
       <c r="H18" t="s">
         <v>17</v>
       </c>
       <c r="L18" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>173</v>
-      </c>
+        <v>372</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" t="s">
         <v>157</v>
       </c>
       <c r="H19" t="s">
         <v>18</v>
       </c>
       <c r="L19" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>174</v>
-      </c>
+        <v>373</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" t="s">
         <v>158</v>
       </c>
       <c r="H20" t="s">
         <v>19</v>
       </c>
       <c r="L20" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>175</v>
-      </c>
+        <v>374</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21" t="s">
+        <v>159</v>
+      </c>
+      <c r="C21" t="s">
         <v>159</v>
       </c>
       <c r="H21" t="s">
         <v>20</v>
       </c>
       <c r="L21" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>176</v>
-      </c>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" t="s">
+        <v>160</v>
+      </c>
+      <c r="C22" t="s">
         <v>160</v>
       </c>
       <c r="H22" t="s">
         <v>21</v>
       </c>
       <c r="L22" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>177</v>
-      </c>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" t="s">
+        <v>161</v>
+      </c>
+      <c r="C23" t="s">
         <v>161</v>
       </c>
       <c r="H23" t="s">
         <v>22</v>
       </c>
       <c r="L23" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>178</v>
-      </c>
+        <v>377</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" t="s">
+        <v>162</v>
+      </c>
+      <c r="C24" t="s">
         <v>162</v>
       </c>
       <c r="H24" t="s">
         <v>23</v>
       </c>
       <c r="L24" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>179</v>
-      </c>
+        <v>378</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" t="s">
+        <v>163</v>
+      </c>
+      <c r="C25" t="s">
         <v>163</v>
       </c>
       <c r="H25" t="s">
         <v>24</v>
       </c>
       <c r="L25" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>180</v>
-      </c>
+        <v>379</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>41</v>
-      </c>
-      <c r="F26" t="s">
+        <v>164</v>
+      </c>
+      <c r="C26" t="s">
         <v>164</v>
       </c>
       <c r="H26" t="s">
         <v>25</v>
       </c>
       <c r="L26" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>181</v>
-      </c>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>42</v>
-      </c>
-      <c r="F27" t="s">
+        <v>165</v>
+      </c>
+      <c r="C27" t="s">
         <v>165</v>
       </c>
       <c r="H27" t="s">
         <v>26</v>
       </c>
       <c r="L27" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>182</v>
-      </c>
+        <v>381</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>43</v>
-      </c>
-      <c r="F28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" t="s">
         <v>166</v>
       </c>
       <c r="H28" t="s">
         <v>27</v>
       </c>
       <c r="L28" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>183</v>
-      </c>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>44</v>
-      </c>
-      <c r="F29" t="s">
+        <v>167</v>
+      </c>
+      <c r="C29" t="s">
         <v>167</v>
       </c>
       <c r="H29" t="s">
         <v>28</v>
       </c>
       <c r="L29" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>184</v>
-      </c>
+        <v>383</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F30" t="s">
+        <v>168</v>
+      </c>
+      <c r="C30" t="s">
         <v>168</v>
       </c>
       <c r="H30" t="s">
         <v>29</v>
       </c>
       <c r="L30" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>185</v>
-      </c>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" t="s">
         <v>169</v>
       </c>
       <c r="H31" t="s">
         <v>30</v>
       </c>
       <c r="L31" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>186</v>
-      </c>
+        <v>385</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" t="s">
+        <v>170</v>
+      </c>
+      <c r="C32" t="s">
         <v>170</v>
       </c>
       <c r="H32" t="s">
         <v>31</v>
       </c>
       <c r="L32" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>187</v>
-      </c>
+        <v>386</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>48</v>
-      </c>
-      <c r="F33" t="s">
+        <v>171</v>
+      </c>
+      <c r="C33" t="s">
         <v>171</v>
       </c>
       <c r="H33" t="s">
         <v>32</v>
       </c>
       <c r="L33" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>188</v>
-      </c>
+        <v>387</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>49</v>
-      </c>
-      <c r="F34" t="s">
+        <v>172</v>
+      </c>
+      <c r="C34" t="s">
         <v>172</v>
       </c>
       <c r="H34" t="s">
         <v>33</v>
       </c>
       <c r="L34" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>189</v>
-      </c>
+        <v>388</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" t="s">
+        <v>173</v>
+      </c>
+      <c r="C35" t="s">
         <v>173</v>
       </c>
       <c r="H35" t="s">
         <v>34</v>
       </c>
       <c r="L35" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>190</v>
-      </c>
+        <v>389</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>51</v>
-      </c>
-      <c r="F36" t="s">
+        <v>174</v>
+      </c>
+      <c r="C36" t="s">
         <v>174</v>
       </c>
       <c r="H36" t="s">
         <v>35</v>
       </c>
       <c r="L36" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>191</v>
-      </c>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>52</v>
-      </c>
-      <c r="F37" t="s">
+        <v>175</v>
+      </c>
+      <c r="C37" t="s">
         <v>175</v>
       </c>
       <c r="H37" t="s">
@@ -2634,32 +2526,26 @@
         <v>295</v>
       </c>
       <c r="L37" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>192</v>
-      </c>
+        <v>391</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F38" t="s">
+        <v>176</v>
+      </c>
+      <c r="C38" t="s">
         <v>176</v>
       </c>
       <c r="H38" t="s">
         <v>37</v>
       </c>
       <c r="L38" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>193</v>
-      </c>
+        <v>392</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>54</v>
+        <v>177</v>
       </c>
       <c r="F39" t="s">
         <v>177</v>
@@ -2668,15 +2554,12 @@
         <v>38</v>
       </c>
       <c r="L39" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>194</v>
-      </c>
+        <v>393</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>55</v>
+        <v>178</v>
       </c>
       <c r="F40" t="s">
         <v>178</v>
@@ -2685,15 +2568,12 @@
         <v>39</v>
       </c>
       <c r="L40" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>195</v>
-      </c>
+        <v>394</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>56</v>
+        <v>179</v>
       </c>
       <c r="F41" t="s">
         <v>179</v>
@@ -2702,15 +2582,12 @@
         <v>40</v>
       </c>
       <c r="L41" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>196</v>
-      </c>
+        <v>395</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>57</v>
+        <v>180</v>
       </c>
       <c r="F42" t="s">
         <v>180</v>
@@ -2722,15 +2599,12 @@
         <v>294</v>
       </c>
       <c r="L42" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>197</v>
-      </c>
+        <v>396</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>58</v>
+        <v>181</v>
       </c>
       <c r="F43" t="s">
         <v>181</v>
@@ -2739,15 +2613,12 @@
         <v>42</v>
       </c>
       <c r="L43" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>198</v>
-      </c>
+        <v>397</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>59</v>
+        <v>182</v>
       </c>
       <c r="F44" t="s">
         <v>182</v>
@@ -2756,15 +2627,12 @@
         <v>43</v>
       </c>
       <c r="L44" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>199</v>
-      </c>
+        <v>398</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>60</v>
+        <v>183</v>
       </c>
       <c r="F45" t="s">
         <v>183</v>
@@ -2773,15 +2641,12 @@
         <v>44</v>
       </c>
       <c r="L45" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>200</v>
-      </c>
+        <v>399</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>61</v>
+        <v>184</v>
       </c>
       <c r="F46" t="s">
         <v>184</v>
@@ -2790,15 +2655,12 @@
         <v>45</v>
       </c>
       <c r="L46" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>201</v>
-      </c>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>62</v>
+        <v>185</v>
       </c>
       <c r="F47" t="s">
         <v>185</v>
@@ -2807,15 +2669,12 @@
         <v>46</v>
       </c>
       <c r="L47" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>202</v>
-      </c>
+        <v>401</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>63</v>
+        <v>186</v>
       </c>
       <c r="F48" t="s">
         <v>186</v>
@@ -2824,15 +2683,12 @@
         <v>47</v>
       </c>
       <c r="L48" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>203</v>
-      </c>
+        <v>402</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>64</v>
+        <v>187</v>
       </c>
       <c r="F49" t="s">
         <v>187</v>
@@ -2841,15 +2697,12 @@
         <v>48</v>
       </c>
       <c r="L49" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>204</v>
-      </c>
+        <v>403</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>65</v>
+        <v>188</v>
       </c>
       <c r="F50" t="s">
         <v>188</v>
@@ -2858,15 +2711,12 @@
         <v>49</v>
       </c>
       <c r="L50" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>205</v>
-      </c>
+        <v>404</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>66</v>
+        <v>189</v>
       </c>
       <c r="F51" t="s">
         <v>189</v>
@@ -2875,15 +2725,12 @@
         <v>50</v>
       </c>
       <c r="L51" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>206</v>
-      </c>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>67</v>
+        <v>190</v>
       </c>
       <c r="F52" t="s">
         <v>190</v>
@@ -2892,15 +2739,12 @@
         <v>51</v>
       </c>
       <c r="L52" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>207</v>
-      </c>
+        <v>406</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>68</v>
+        <v>191</v>
       </c>
       <c r="F53" t="s">
         <v>191</v>
@@ -2909,15 +2753,12 @@
         <v>52</v>
       </c>
       <c r="L53" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>208</v>
-      </c>
+        <v>407</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>69</v>
+        <v>192</v>
       </c>
       <c r="F54" t="s">
         <v>192</v>
@@ -2926,15 +2767,12 @@
         <v>53</v>
       </c>
       <c r="L54" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>209</v>
-      </c>
+        <v>408</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>70</v>
+        <v>193</v>
       </c>
       <c r="F55" t="s">
         <v>193</v>
@@ -2943,15 +2781,12 @@
         <v>54</v>
       </c>
       <c r="L55" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>210</v>
-      </c>
+        <v>409</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>71</v>
+        <v>194</v>
       </c>
       <c r="F56" t="s">
         <v>194</v>
@@ -2960,15 +2795,12 @@
         <v>55</v>
       </c>
       <c r="L56" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>211</v>
-      </c>
+        <v>410</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>72</v>
+        <v>195</v>
       </c>
       <c r="F57" t="s">
         <v>195</v>
@@ -2977,15 +2809,12 @@
         <v>56</v>
       </c>
       <c r="L57" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>212</v>
-      </c>
+        <v>411</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>73</v>
+        <v>196</v>
       </c>
       <c r="F58" t="s">
         <v>196</v>
@@ -2994,15 +2823,12 @@
         <v>57</v>
       </c>
       <c r="L58" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>213</v>
-      </c>
+        <v>412</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>74</v>
+        <v>197</v>
       </c>
       <c r="F59" t="s">
         <v>197</v>
@@ -3011,15 +2837,12 @@
         <v>58</v>
       </c>
       <c r="L59" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>214</v>
-      </c>
+        <v>413</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>75</v>
+        <v>198</v>
       </c>
       <c r="F60" t="s">
         <v>198</v>
@@ -3028,15 +2851,12 @@
         <v>59</v>
       </c>
       <c r="L60" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>215</v>
-      </c>
+        <v>414</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>76</v>
+        <v>199</v>
       </c>
       <c r="F61" t="s">
         <v>199</v>
@@ -3045,15 +2865,12 @@
         <v>60</v>
       </c>
       <c r="L61" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>216</v>
-      </c>
+        <v>415</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>77</v>
+        <v>200</v>
       </c>
       <c r="F62" t="s">
         <v>200</v>
@@ -3062,15 +2879,12 @@
         <v>61</v>
       </c>
       <c r="L62" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>217</v>
-      </c>
+        <v>416</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>78</v>
+        <v>201</v>
       </c>
       <c r="F63" t="s">
         <v>201</v>
@@ -3079,15 +2893,12 @@
         <v>62</v>
       </c>
       <c r="L63" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>218</v>
-      </c>
+        <v>417</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>79</v>
+        <v>202</v>
       </c>
       <c r="F64" t="s">
         <v>202</v>
@@ -3096,15 +2907,12 @@
         <v>63</v>
       </c>
       <c r="L64" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>219</v>
-      </c>
+        <v>418</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>80</v>
+        <v>203</v>
       </c>
       <c r="F65" t="s">
         <v>203</v>
@@ -3113,15 +2921,12 @@
         <v>64</v>
       </c>
       <c r="L65" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>220</v>
-      </c>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>81</v>
+        <v>204</v>
       </c>
       <c r="F66" t="s">
         <v>204</v>
@@ -3130,15 +2935,12 @@
         <v>65</v>
       </c>
       <c r="L66" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>221</v>
-      </c>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>82</v>
+        <v>205</v>
       </c>
       <c r="F67" t="s">
         <v>205</v>
@@ -3147,15 +2949,12 @@
         <v>66</v>
       </c>
       <c r="L67" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>222</v>
-      </c>
+        <v>421</v>
+      </c>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>83</v>
+        <v>206</v>
       </c>
       <c r="F68" t="s">
         <v>206</v>
@@ -3164,15 +2963,12 @@
         <v>67</v>
       </c>
       <c r="L68" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>223</v>
-      </c>
+        <v>422</v>
+      </c>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>84</v>
+        <v>207</v>
       </c>
       <c r="F69" t="s">
         <v>207</v>
@@ -3181,15 +2977,12 @@
         <v>68</v>
       </c>
       <c r="L69" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>224</v>
-      </c>
+        <v>423</v>
+      </c>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>85</v>
+        <v>208</v>
       </c>
       <c r="F70" t="s">
         <v>208</v>
@@ -3198,15 +2991,12 @@
         <v>69</v>
       </c>
       <c r="L70" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>225</v>
-      </c>
+        <v>424</v>
+      </c>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>86</v>
+        <v>209</v>
       </c>
       <c r="F71" t="s">
         <v>209</v>
@@ -3215,15 +3005,12 @@
         <v>70</v>
       </c>
       <c r="L71" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>226</v>
-      </c>
+        <v>425</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>87</v>
+        <v>210</v>
       </c>
       <c r="F72" t="s">
         <v>210</v>
@@ -3232,15 +3019,12 @@
         <v>71</v>
       </c>
       <c r="L72" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>227</v>
-      </c>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>88</v>
+        <v>211</v>
       </c>
       <c r="F73" t="s">
         <v>211</v>
@@ -3249,15 +3033,12 @@
         <v>72</v>
       </c>
       <c r="L73" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>228</v>
-      </c>
+        <v>427</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>89</v>
+        <v>212</v>
       </c>
       <c r="F74" t="s">
         <v>212</v>
@@ -3266,15 +3047,12 @@
         <v>73</v>
       </c>
       <c r="L74" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>229</v>
-      </c>
+        <v>428</v>
+      </c>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>90</v>
+        <v>213</v>
       </c>
       <c r="F75" t="s">
         <v>213</v>
@@ -3283,15 +3061,12 @@
         <v>74</v>
       </c>
       <c r="L75" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>230</v>
-      </c>
+        <v>429</v>
+      </c>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>91</v>
+        <v>214</v>
       </c>
       <c r="F76" t="s">
         <v>214</v>
@@ -3300,15 +3075,12 @@
         <v>75</v>
       </c>
       <c r="L76" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>231</v>
-      </c>
+        <v>430</v>
+      </c>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>92</v>
+        <v>215</v>
       </c>
       <c r="F77" t="s">
         <v>215</v>
@@ -3317,15 +3089,12 @@
         <v>76</v>
       </c>
       <c r="L77" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>232</v>
-      </c>
+        <v>431</v>
+      </c>
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>93</v>
+        <v>216</v>
       </c>
       <c r="F78" t="s">
         <v>216</v>
@@ -3334,15 +3103,12 @@
         <v>77</v>
       </c>
       <c r="L78" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>233</v>
-      </c>
+        <v>432</v>
+      </c>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>94</v>
+        <v>217</v>
       </c>
       <c r="F79" t="s">
         <v>217</v>
@@ -3351,15 +3117,12 @@
         <v>78</v>
       </c>
       <c r="L79" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>234</v>
-      </c>
+        <v>433</v>
+      </c>
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>95</v>
+        <v>218</v>
       </c>
       <c r="F80" t="s">
         <v>218</v>
@@ -3368,15 +3131,12 @@
         <v>79</v>
       </c>
       <c r="L80" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>235</v>
-      </c>
+        <v>434</v>
+      </c>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>96</v>
+        <v>219</v>
       </c>
       <c r="F81" t="s">
         <v>219</v>
@@ -3385,15 +3145,12 @@
         <v>80</v>
       </c>
       <c r="L81" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>236</v>
-      </c>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>97</v>
+        <v>220</v>
       </c>
       <c r="F82" t="s">
         <v>220</v>
@@ -3402,15 +3159,12 @@
         <v>81</v>
       </c>
       <c r="L82" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>237</v>
-      </c>
+        <v>436</v>
+      </c>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>98</v>
+        <v>221</v>
       </c>
       <c r="F83" t="s">
         <v>221</v>
@@ -3419,15 +3173,12 @@
         <v>82</v>
       </c>
       <c r="L83" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>238</v>
-      </c>
+        <v>437</v>
+      </c>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>99</v>
+        <v>222</v>
       </c>
       <c r="F84" t="s">
         <v>222</v>
@@ -3436,15 +3187,12 @@
         <v>83</v>
       </c>
       <c r="L84" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>239</v>
-      </c>
+        <v>438</v>
+      </c>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>100</v>
+        <v>223</v>
       </c>
       <c r="F85" t="s">
         <v>223</v>
@@ -3453,15 +3201,12 @@
         <v>84</v>
       </c>
       <c r="L85" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>240</v>
-      </c>
+        <v>439</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>101</v>
+        <v>224</v>
       </c>
       <c r="F86" t="s">
         <v>224</v>
@@ -3470,15 +3215,12 @@
         <v>85</v>
       </c>
       <c r="L86" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>241</v>
-      </c>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>102</v>
+        <v>225</v>
       </c>
       <c r="F87" t="s">
         <v>225</v>
@@ -3487,15 +3229,12 @@
         <v>86</v>
       </c>
       <c r="L87" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>242</v>
-      </c>
+        <v>441</v>
+      </c>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>103</v>
+        <v>226</v>
       </c>
       <c r="F88" t="s">
         <v>226</v>
@@ -3504,15 +3243,12 @@
         <v>87</v>
       </c>
       <c r="L88" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>243</v>
-      </c>
+        <v>442</v>
+      </c>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>104</v>
+        <v>227</v>
       </c>
       <c r="F89" t="s">
         <v>227</v>
@@ -3521,15 +3257,12 @@
         <v>88</v>
       </c>
       <c r="L89" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>244</v>
-      </c>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>105</v>
+        <v>228</v>
       </c>
       <c r="F90" t="s">
         <v>228</v>
@@ -3538,15 +3271,12 @@
         <v>89</v>
       </c>
       <c r="L90" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>245</v>
-      </c>
+        <v>444</v>
+      </c>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>106</v>
+        <v>229</v>
       </c>
       <c r="F91" t="s">
         <v>229</v>
@@ -3555,15 +3285,12 @@
         <v>90</v>
       </c>
       <c r="L91" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>246</v>
-      </c>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>107</v>
+        <v>230</v>
       </c>
       <c r="F92" t="s">
         <v>230</v>
@@ -3572,15 +3299,12 @@
         <v>91</v>
       </c>
       <c r="L92" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>247</v>
-      </c>
+        <v>446</v>
+      </c>
+    </row>
+    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>108</v>
+        <v>231</v>
       </c>
       <c r="F93" t="s">
         <v>231</v>
@@ -3589,15 +3313,12 @@
         <v>92</v>
       </c>
       <c r="L93" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>248</v>
-      </c>
+        <v>447</v>
+      </c>
+    </row>
+    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>109</v>
+        <v>232</v>
       </c>
       <c r="F94" t="s">
         <v>232</v>
@@ -3606,15 +3327,12 @@
         <v>93</v>
       </c>
       <c r="L94" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>249</v>
-      </c>
+        <v>448</v>
+      </c>
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>110</v>
+        <v>233</v>
       </c>
       <c r="F95" t="s">
         <v>233</v>
@@ -3623,15 +3341,12 @@
         <v>94</v>
       </c>
       <c r="L95" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>250</v>
-      </c>
+        <v>449</v>
+      </c>
+    </row>
+    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>111</v>
+        <v>234</v>
       </c>
       <c r="F96" t="s">
         <v>234</v>
@@ -3640,15 +3355,12 @@
         <v>95</v>
       </c>
       <c r="L96" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>251</v>
-      </c>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>112</v>
+        <v>235</v>
       </c>
       <c r="F97" t="s">
         <v>235</v>
@@ -3657,15 +3369,12 @@
         <v>96</v>
       </c>
       <c r="L97" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>252</v>
-      </c>
+        <v>451</v>
+      </c>
+    </row>
+    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>113</v>
+        <v>236</v>
       </c>
       <c r="F98" t="s">
         <v>236</v>
@@ -3674,18 +3383,15 @@
         <v>97</v>
       </c>
       <c r="I98" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="L98" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>253</v>
-      </c>
+        <v>452</v>
+      </c>
+    </row>
+    <row r="99" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>114</v>
+        <v>237</v>
       </c>
       <c r="F99" t="s">
         <v>237</v>
@@ -3694,18 +3400,15 @@
         <v>98</v>
       </c>
       <c r="I99" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="L99" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>254</v>
-      </c>
+        <v>453</v>
+      </c>
+    </row>
+    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>115</v>
+        <v>238</v>
       </c>
       <c r="F100" t="s">
         <v>238</v>
@@ -3714,18 +3417,15 @@
         <v>99</v>
       </c>
       <c r="I100" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="L100" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>255</v>
-      </c>
+        <v>454</v>
+      </c>
+    </row>
+    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>116</v>
+        <v>239</v>
       </c>
       <c r="F101" t="s">
         <v>239</v>
@@ -3734,18 +3434,15 @@
         <v>100</v>
       </c>
       <c r="I101" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="L101" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>256</v>
-      </c>
+        <v>455</v>
+      </c>
+    </row>
+    <row r="102" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>117</v>
+        <v>240</v>
       </c>
       <c r="F102" t="s">
         <v>240</v>
@@ -3754,18 +3451,15 @@
         <v>101</v>
       </c>
       <c r="I102" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="L102" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>257</v>
-      </c>
+        <v>456</v>
+      </c>
+    </row>
+    <row r="103" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>118</v>
+        <v>241</v>
       </c>
       <c r="F103" t="s">
         <v>241</v>
@@ -3774,18 +3468,15 @@
         <v>102</v>
       </c>
       <c r="I103" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="L103" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>258</v>
-      </c>
+        <v>457</v>
+      </c>
+    </row>
+    <row r="104" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>119</v>
+        <v>242</v>
       </c>
       <c r="F104" t="s">
         <v>242</v>
@@ -3794,15 +3485,12 @@
         <v>103</v>
       </c>
       <c r="L104" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>259</v>
-      </c>
+        <v>458</v>
+      </c>
+    </row>
+    <row r="105" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>120</v>
+        <v>243</v>
       </c>
       <c r="F105" t="s">
         <v>243</v>
@@ -3811,18 +3499,15 @@
         <v>104</v>
       </c>
       <c r="I105" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="L105" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>260</v>
-      </c>
+        <v>459</v>
+      </c>
+    </row>
+    <row r="106" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>121</v>
+        <v>244</v>
       </c>
       <c r="F106" t="s">
         <v>244</v>
@@ -3831,15 +3516,12 @@
         <v>105</v>
       </c>
       <c r="L106" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>261</v>
-      </c>
+        <v>460</v>
+      </c>
+    </row>
+    <row r="107" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>122</v>
+        <v>245</v>
       </c>
       <c r="F107" t="s">
         <v>245</v>
@@ -3848,18 +3530,15 @@
         <v>106</v>
       </c>
       <c r="I107" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="L107" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>262</v>
-      </c>
+        <v>461</v>
+      </c>
+    </row>
+    <row r="108" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>123</v>
+        <v>246</v>
       </c>
       <c r="F108" t="s">
         <v>246</v>
@@ -3868,15 +3547,12 @@
         <v>107</v>
       </c>
       <c r="L108" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>263</v>
-      </c>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="109" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>124</v>
+        <v>247</v>
       </c>
       <c r="F109" t="s">
         <v>247</v>
@@ -3885,18 +3561,15 @@
         <v>108</v>
       </c>
       <c r="I109" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="L109" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>264</v>
-      </c>
+        <v>463</v>
+      </c>
+    </row>
+    <row r="110" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>125</v>
+        <v>248</v>
       </c>
       <c r="F110" t="s">
         <v>248</v>
@@ -3905,18 +3578,15 @@
         <v>109</v>
       </c>
       <c r="I110" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="L110" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>265</v>
-      </c>
+        <v>464</v>
+      </c>
+    </row>
+    <row r="111" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>126</v>
+        <v>249</v>
       </c>
       <c r="F111" t="s">
         <v>249</v>
@@ -3925,18 +3595,15 @@
         <v>110</v>
       </c>
       <c r="I111" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="L111" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>266</v>
-      </c>
+        <v>465</v>
+      </c>
+    </row>
+    <row r="112" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>127</v>
+        <v>250</v>
       </c>
       <c r="F112" t="s">
         <v>250</v>
@@ -3945,15 +3612,12 @@
         <v>111</v>
       </c>
       <c r="L112" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>267</v>
-      </c>
+        <v>466</v>
+      </c>
+    </row>
+    <row r="113" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>128</v>
+        <v>251</v>
       </c>
       <c r="F113" t="s">
         <v>251</v>
@@ -3962,18 +3626,15 @@
         <v>112</v>
       </c>
       <c r="I113" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="L113" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>268</v>
-      </c>
+        <v>467</v>
+      </c>
+    </row>
+    <row r="114" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>129</v>
+        <v>252</v>
       </c>
       <c r="F114" t="s">
         <v>252</v>
@@ -3982,15 +3643,12 @@
         <v>113</v>
       </c>
       <c r="L114" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>269</v>
-      </c>
+        <v>468</v>
+      </c>
+    </row>
+    <row r="115" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>130</v>
+        <v>253</v>
       </c>
       <c r="F115" t="s">
         <v>253</v>
@@ -3999,15 +3657,12 @@
         <v>114</v>
       </c>
       <c r="L115" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>270</v>
-      </c>
+        <v>469</v>
+      </c>
+    </row>
+    <row r="116" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>131</v>
+        <v>254</v>
       </c>
       <c r="F116" t="s">
         <v>254</v>
@@ -4016,15 +3671,12 @@
         <v>115</v>
       </c>
       <c r="L116" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>271</v>
-      </c>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="117" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>132</v>
+        <v>255</v>
       </c>
       <c r="F117" t="s">
         <v>255</v>
@@ -4033,15 +3685,12 @@
         <v>116</v>
       </c>
       <c r="L117" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>272</v>
-      </c>
+        <v>471</v>
+      </c>
+    </row>
+    <row r="118" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>133</v>
+        <v>256</v>
       </c>
       <c r="F118" t="s">
         <v>256</v>
@@ -4050,15 +3699,12 @@
         <v>117</v>
       </c>
       <c r="L118" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>273</v>
-      </c>
+        <v>472</v>
+      </c>
+    </row>
+    <row r="119" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>134</v>
+        <v>257</v>
       </c>
       <c r="F119" t="s">
         <v>257</v>
@@ -4067,15 +3713,12 @@
         <v>118</v>
       </c>
       <c r="L119" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>274</v>
-      </c>
+        <v>473</v>
+      </c>
+    </row>
+    <row r="120" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>135</v>
+        <v>258</v>
       </c>
       <c r="F120" t="s">
         <v>258</v>
@@ -4084,15 +3727,12 @@
         <v>119</v>
       </c>
       <c r="L120" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>275</v>
-      </c>
+        <v>474</v>
+      </c>
+    </row>
+    <row r="121" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>136</v>
+        <v>259</v>
       </c>
       <c r="F121" t="s">
         <v>259</v>
@@ -4101,15 +3741,12 @@
         <v>120</v>
       </c>
       <c r="L121" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>276</v>
-      </c>
+        <v>475</v>
+      </c>
+    </row>
+    <row r="122" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>137</v>
+        <v>260</v>
       </c>
       <c r="F122" t="s">
         <v>260</v>
@@ -4118,15 +3755,12 @@
         <v>121</v>
       </c>
       <c r="L122" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>277</v>
-      </c>
+        <v>476</v>
+      </c>
+    </row>
+    <row r="123" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>138</v>
+        <v>261</v>
       </c>
       <c r="F123" t="s">
         <v>261</v>
@@ -4135,15 +3769,12 @@
         <v>122</v>
       </c>
       <c r="L123" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>278</v>
-      </c>
+        <v>477</v>
+      </c>
+    </row>
+    <row r="124" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>139</v>
+        <v>262</v>
       </c>
       <c r="F124" t="s">
         <v>262</v>
@@ -4152,15 +3783,12 @@
         <v>123</v>
       </c>
       <c r="L124" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>279</v>
-      </c>
+        <v>478</v>
+      </c>
+    </row>
+    <row r="125" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>140</v>
+        <v>263</v>
       </c>
       <c r="F125" t="s">
         <v>263</v>
@@ -4169,15 +3797,12 @@
         <v>124</v>
       </c>
       <c r="L125" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>280</v>
-      </c>
+        <v>479</v>
+      </c>
+    </row>
+    <row r="126" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>141</v>
+        <v>264</v>
       </c>
       <c r="F126" t="s">
         <v>264</v>
@@ -4186,15 +3811,12 @@
         <v>125</v>
       </c>
       <c r="L126" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>281</v>
-      </c>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="127" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>142</v>
+        <v>265</v>
       </c>
       <c r="F127" t="s">
         <v>265</v>
@@ -4203,15 +3825,12 @@
         <v>126</v>
       </c>
       <c r="L127" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>282</v>
-      </c>
+        <v>481</v>
+      </c>
+    </row>
+    <row r="128" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>143</v>
+        <v>266</v>
       </c>
       <c r="F128" t="s">
         <v>266</v>
@@ -4220,15 +3839,12 @@
         <v>127</v>
       </c>
       <c r="L128" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>283</v>
-      </c>
+        <v>482</v>
+      </c>
+    </row>
+    <row r="129" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>144</v>
+        <v>267</v>
       </c>
       <c r="F129" t="s">
         <v>267</v>
@@ -4237,15 +3853,12 @@
         <v>128</v>
       </c>
       <c r="L129" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>284</v>
-      </c>
+        <v>483</v>
+      </c>
+    </row>
+    <row r="130" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>145</v>
+        <v>268</v>
       </c>
       <c r="F130" t="s">
         <v>268</v>
@@ -4254,15 +3867,12 @@
         <v>129</v>
       </c>
       <c r="L130" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>285</v>
-      </c>
+        <v>484</v>
+      </c>
+    </row>
+    <row r="131" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>146</v>
+        <v>269</v>
       </c>
       <c r="F131" t="s">
         <v>269</v>
@@ -4271,15 +3881,12 @@
         <v>130</v>
       </c>
       <c r="L131" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>286</v>
-      </c>
+        <v>485</v>
+      </c>
+    </row>
+    <row r="132" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>147</v>
+        <v>270</v>
       </c>
       <c r="F132" t="s">
         <v>270</v>
@@ -4288,15 +3895,12 @@
         <v>131</v>
       </c>
       <c r="L132" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>287</v>
-      </c>
+        <v>486</v>
+      </c>
+    </row>
+    <row r="133" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>148</v>
+        <v>271</v>
       </c>
       <c r="F133" t="s">
         <v>271</v>
@@ -4308,12 +3912,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>288</v>
-      </c>
+    <row r="134" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>149</v>
+        <v>272</v>
       </c>
       <c r="F134" t="s">
         <v>272</v>
@@ -4325,12 +3926,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>289</v>
-      </c>
+    <row r="135" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>150</v>
+        <v>273</v>
       </c>
       <c r="F135" t="s">
         <v>273</v>
@@ -4342,12 +3940,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>290</v>
-      </c>
+    <row r="136" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>151</v>
+        <v>274</v>
       </c>
       <c r="F136" t="s">
         <v>274</v>
@@ -4359,12 +3954,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>291</v>
-      </c>
+    <row r="137" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>152</v>
+        <v>275</v>
       </c>
       <c r="F137" t="s">
         <v>275</v>
@@ -4373,15 +3965,12 @@
         <v>136</v>
       </c>
       <c r="L137" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>292</v>
-      </c>
+        <v>487</v>
+      </c>
+    </row>
+    <row r="138" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>153</v>
+        <v>276</v>
       </c>
       <c r="F138" t="s">
         <v>276</v>
@@ -4390,15 +3979,12 @@
         <v>137</v>
       </c>
       <c r="L138" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>293</v>
-      </c>
+        <v>488</v>
+      </c>
+    </row>
+    <row r="139" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>154</v>
+        <v>277</v>
       </c>
       <c r="F139" t="s">
         <v>277</v>
@@ -4407,10 +3993,13 @@
         <v>138</v>
       </c>
       <c r="L139" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="140" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>278</v>
+      </c>
       <c r="F140" t="s">
         <v>278</v>
       </c>
@@ -4418,15 +4007,12 @@
         <v>139</v>
       </c>
       <c r="L140" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>296</v>
-      </c>
+        <v>490</v>
+      </c>
+    </row>
+    <row r="141" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>326</v>
+        <v>279</v>
       </c>
       <c r="F141" t="s">
         <v>279</v>
@@ -4435,15 +4021,12 @@
         <v>140</v>
       </c>
       <c r="L141" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>297</v>
-      </c>
+        <v>491</v>
+      </c>
+    </row>
+    <row r="142" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>327</v>
+        <v>280</v>
       </c>
       <c r="F142" t="s">
         <v>280</v>
@@ -4452,15 +4035,12 @@
         <v>141</v>
       </c>
       <c r="L142" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>298</v>
-      </c>
+        <v>492</v>
+      </c>
+    </row>
+    <row r="143" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>328</v>
+        <v>281</v>
       </c>
       <c r="F143" t="s">
         <v>281</v>
@@ -4469,15 +4049,12 @@
         <v>142</v>
       </c>
       <c r="L143" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>299</v>
-      </c>
+        <v>493</v>
+      </c>
+    </row>
+    <row r="144" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>329</v>
+        <v>282</v>
       </c>
       <c r="F144" t="s">
         <v>282</v>
@@ -4486,15 +4063,12 @@
         <v>143</v>
       </c>
       <c r="L144" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>300</v>
-      </c>
       <c r="B145" t="s">
-        <v>330</v>
+        <v>283</v>
       </c>
       <c r="F145" t="s">
         <v>283</v>
@@ -4507,11 +4081,8 @@
       </c>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>301</v>
-      </c>
       <c r="B146" t="s">
-        <v>331</v>
+        <v>284</v>
       </c>
       <c r="F146" t="s">
         <v>284</v>
@@ -4524,11 +4095,8 @@
       </c>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>302</v>
-      </c>
       <c r="B147" t="s">
-        <v>332</v>
+        <v>285</v>
       </c>
       <c r="F147" t="s">
         <v>285</v>
@@ -4537,15 +4105,12 @@
         <v>146</v>
       </c>
       <c r="L147" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>303</v>
-      </c>
       <c r="B148" t="s">
-        <v>333</v>
+        <v>286</v>
       </c>
       <c r="F148" t="s">
         <v>286</v>
@@ -4554,15 +4119,12 @@
         <v>147</v>
       </c>
       <c r="L148" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>304</v>
-      </c>
       <c r="B149" t="s">
-        <v>334</v>
+        <v>287</v>
       </c>
       <c r="F149" t="s">
         <v>287</v>
@@ -4571,15 +4133,12 @@
         <v>148</v>
       </c>
       <c r="L149" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>305</v>
-      </c>
       <c r="B150" t="s">
-        <v>335</v>
+        <v>288</v>
       </c>
       <c r="F150" t="s">
         <v>288</v>
@@ -4588,15 +4147,12 @@
         <v>149</v>
       </c>
       <c r="L150" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>306</v>
-      </c>
       <c r="B151" t="s">
-        <v>336</v>
+        <v>289</v>
       </c>
       <c r="F151" t="s">
         <v>289</v>
@@ -4606,11 +4162,8 @@
       </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>307</v>
-      </c>
       <c r="B152" t="s">
-        <v>337</v>
+        <v>290</v>
       </c>
       <c r="F152" t="s">
         <v>290</v>
@@ -4620,11 +4173,8 @@
       </c>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>308</v>
-      </c>
       <c r="B153" t="s">
-        <v>338</v>
+        <v>291</v>
       </c>
       <c r="F153" t="s">
         <v>291</v>
@@ -4634,11 +4184,8 @@
       </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>309</v>
-      </c>
       <c r="B154" t="s">
-        <v>339</v>
+        <v>292</v>
       </c>
       <c r="F154" t="s">
         <v>292</v>
@@ -4648,11 +4195,8 @@
       </c>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>310</v>
-      </c>
       <c r="B155" t="s">
-        <v>340</v>
+        <v>293</v>
       </c>
       <c r="F155" t="s">
         <v>293</v>
@@ -4663,612 +4207,425 @@
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
+        <v>2</v>
+      </c>
+      <c r="F156" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F157" t="s">
+        <v>297</v>
+      </c>
+      <c r="H157" t="s">
+        <v>327</v>
+      </c>
+      <c r="J157" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F158" t="s">
+        <v>298</v>
+      </c>
+      <c r="H158" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F159" t="s">
+        <v>299</v>
+      </c>
+      <c r="H159" t="s">
+        <v>329</v>
+      </c>
+      <c r="J159" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F160" t="s">
+        <v>300</v>
+      </c>
+      <c r="H160" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="161" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F161" t="s">
+        <v>301</v>
+      </c>
+      <c r="H161" t="s">
+        <v>331</v>
+      </c>
+      <c r="J161" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="162" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F162" t="s">
+        <v>302</v>
+      </c>
+      <c r="H162" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="163" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F163" t="s">
+        <v>303</v>
+      </c>
+      <c r="H163" t="s">
+        <v>333</v>
+      </c>
+      <c r="J163" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="164" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F164" t="s">
+        <v>304</v>
+      </c>
+      <c r="H164" t="s">
+        <v>334</v>
+      </c>
+      <c r="J164" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="165" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F165" t="s">
+        <v>305</v>
+      </c>
+      <c r="H165" t="s">
+        <v>335</v>
+      </c>
+      <c r="J165" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="166" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F166" t="s">
+        <v>306</v>
+      </c>
+      <c r="H166" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="167" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F167" t="s">
+        <v>307</v>
+      </c>
+      <c r="H167" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="168" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F168" t="s">
+        <v>308</v>
+      </c>
+      <c r="H168" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="169" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F169" t="s">
+        <v>309</v>
+      </c>
+      <c r="H169" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="170" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F170" t="s">
+        <v>310</v>
+      </c>
+      <c r="H170" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="171" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F171" t="s">
         <v>311</v>
       </c>
-      <c r="B156" t="s">
+      <c r="H171" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+    <row r="172" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F172" t="s">
         <v>312</v>
       </c>
-      <c r="B157" t="s">
+      <c r="H172" t="s">
         <v>342</v>
       </c>
-      <c r="F157" t="s">
-        <v>296</v>
-      </c>
-      <c r="H157" t="s">
+    </row>
+    <row r="173" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F173" t="s">
+        <v>313</v>
+      </c>
+      <c r="H173" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="174" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F174" t="s">
+        <v>314</v>
+      </c>
+      <c r="H174" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="175" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F175" t="s">
+        <v>315</v>
+      </c>
+      <c r="H175" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="176" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F176" t="s">
+        <v>316</v>
+      </c>
+      <c r="H176" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="177" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F177" t="s">
+        <v>317</v>
+      </c>
+      <c r="H177" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="178" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F178" t="s">
+        <v>318</v>
+      </c>
+      <c r="H178" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="179" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F179" t="s">
+        <v>319</v>
+      </c>
+      <c r="H179" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="180" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F180" t="s">
+        <v>320</v>
+      </c>
+      <c r="H180" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="181" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F181" t="s">
+        <v>321</v>
+      </c>
+      <c r="H181" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="182" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F182" t="s">
+        <v>322</v>
+      </c>
+      <c r="H182" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="183" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F183" t="s">
+        <v>323</v>
+      </c>
+      <c r="H183" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="184" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F184" t="s">
+        <v>324</v>
+      </c>
+      <c r="H184" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="185" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F185" t="s">
+        <v>325</v>
+      </c>
+      <c r="H185" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="186" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F186" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>313</v>
-      </c>
-      <c r="B158" t="s">
-        <v>343</v>
-      </c>
-      <c r="F158" t="s">
-        <v>297</v>
-      </c>
-      <c r="H158" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>314</v>
-      </c>
-      <c r="B159" t="s">
-        <v>344</v>
-      </c>
-      <c r="F159" t="s">
-        <v>298</v>
-      </c>
-      <c r="H159" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>315</v>
-      </c>
-      <c r="B160" t="s">
-        <v>345</v>
-      </c>
-      <c r="F160" t="s">
-        <v>299</v>
-      </c>
-      <c r="H160" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>316</v>
-      </c>
-      <c r="B161" t="s">
-        <v>346</v>
-      </c>
-      <c r="F161" t="s">
-        <v>300</v>
-      </c>
-      <c r="H161" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>317</v>
-      </c>
-      <c r="B162" t="s">
-        <v>347</v>
-      </c>
-      <c r="F162" t="s">
-        <v>301</v>
-      </c>
-      <c r="H162" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>318</v>
-      </c>
-      <c r="B163" t="s">
-        <v>348</v>
-      </c>
-      <c r="F163" t="s">
-        <v>302</v>
-      </c>
-      <c r="H163" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>319</v>
-      </c>
-      <c r="B164" t="s">
-        <v>349</v>
-      </c>
-      <c r="F164" t="s">
-        <v>303</v>
-      </c>
-      <c r="H164" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>320</v>
-      </c>
-      <c r="B165" t="s">
-        <v>350</v>
-      </c>
-      <c r="F165" t="s">
-        <v>304</v>
-      </c>
-      <c r="H165" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>321</v>
-      </c>
-      <c r="B166" t="s">
-        <v>351</v>
-      </c>
-      <c r="F166" t="s">
-        <v>305</v>
-      </c>
-      <c r="H166" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>322</v>
-      </c>
-      <c r="B167" t="s">
-        <v>352</v>
-      </c>
-      <c r="F167" t="s">
-        <v>306</v>
-      </c>
-      <c r="H167" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>323</v>
-      </c>
-      <c r="B168" t="s">
-        <v>353</v>
-      </c>
-      <c r="F168" t="s">
-        <v>307</v>
-      </c>
-      <c r="H168" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>324</v>
-      </c>
-      <c r="B169" t="s">
-        <v>354</v>
-      </c>
-      <c r="F169" t="s">
-        <v>308</v>
-      </c>
-      <c r="H169" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>325</v>
-      </c>
-      <c r="B170" t="s">
-        <v>355</v>
-      </c>
-      <c r="F170" t="s">
-        <v>309</v>
-      </c>
-      <c r="H170" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F171" t="s">
-        <v>310</v>
-      </c>
-      <c r="H171" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F172" t="s">
-        <v>311</v>
-      </c>
-      <c r="H172" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F173" t="s">
-        <v>312</v>
-      </c>
-      <c r="H173" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>158</v>
-      </c>
-      <c r="B174" t="s">
-        <v>516</v>
-      </c>
-      <c r="F174" t="s">
-        <v>313</v>
-      </c>
-      <c r="H174" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>159</v>
-      </c>
-      <c r="B175" t="s">
-        <v>517</v>
-      </c>
-      <c r="F175" t="s">
-        <v>314</v>
-      </c>
-      <c r="H175" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>160</v>
-      </c>
-      <c r="B176" t="s">
-        <v>518</v>
-      </c>
-      <c r="F176" t="s">
-        <v>315</v>
-      </c>
-      <c r="H176" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>161</v>
-      </c>
-      <c r="B177" t="s">
-        <v>519</v>
-      </c>
-      <c r="F177" t="s">
-        <v>316</v>
-      </c>
-      <c r="H177" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>511</v>
-      </c>
-      <c r="B178" t="s">
-        <v>520</v>
-      </c>
-      <c r="F178" t="s">
-        <v>317</v>
-      </c>
-      <c r="H178" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>168</v>
-      </c>
-      <c r="B179" t="s">
-        <v>521</v>
-      </c>
-      <c r="F179" t="s">
-        <v>318</v>
-      </c>
-      <c r="H179" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>512</v>
-      </c>
-      <c r="B180" t="s">
-        <v>522</v>
-      </c>
-      <c r="F180" t="s">
-        <v>319</v>
-      </c>
-      <c r="H180" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>513</v>
-      </c>
-      <c r="B181" t="s">
-        <v>523</v>
-      </c>
-      <c r="F181" t="s">
-        <v>320</v>
-      </c>
-      <c r="H181" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>207</v>
-      </c>
-      <c r="B182" t="s">
-        <v>524</v>
-      </c>
-      <c r="F182" t="s">
-        <v>321</v>
-      </c>
-      <c r="H182" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>208</v>
-      </c>
-      <c r="B183" t="s">
+      <c r="H186" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="187" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F187" t="s">
         <v>525</v>
       </c>
-      <c r="F183" t="s">
-        <v>322</v>
-      </c>
-      <c r="H183" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>209</v>
-      </c>
-      <c r="B184" t="s">
-        <v>526</v>
-      </c>
-      <c r="F184" t="s">
-        <v>323</v>
-      </c>
-      <c r="H184" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>215</v>
-      </c>
-      <c r="B185" t="s">
-        <v>527</v>
-      </c>
-      <c r="F185" t="s">
-        <v>324</v>
-      </c>
-      <c r="H185" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>514</v>
-      </c>
-      <c r="B186" t="s">
-        <v>528</v>
-      </c>
-      <c r="F186" t="s">
-        <v>325</v>
-      </c>
-      <c r="H186" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>225</v>
-      </c>
-      <c r="B187" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>226</v>
-      </c>
-      <c r="B188" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>515</v>
-      </c>
-      <c r="B189" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>287</v>
-      </c>
-      <c r="B190" t="s">
-        <v>532</v>
-      </c>
+    </row>
+    <row r="190" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F190" t="s">
         <v>158</v>
       </c>
       <c r="H190" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>288</v>
-      </c>
-      <c r="B191" t="s">
-        <v>533</v>
-      </c>
+        <v>526</v>
+      </c>
+    </row>
+    <row r="191" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F191" t="s">
         <v>159</v>
       </c>
       <c r="H191" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>289</v>
-      </c>
-      <c r="B192" t="s">
-        <v>534</v>
-      </c>
+        <v>527</v>
+      </c>
+    </row>
+    <row r="192" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F192" t="s">
         <v>160</v>
       </c>
       <c r="H192" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>290</v>
-      </c>
-      <c r="B193" t="s">
-        <v>535</v>
-      </c>
+        <v>528</v>
+      </c>
+    </row>
+    <row r="193" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F193" t="s">
         <v>161</v>
       </c>
       <c r="H193" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="194" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F194" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
       <c r="H194" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="195" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F195" t="s">
         <v>168</v>
       </c>
       <c r="H195" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="196" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F196" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="H196" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="197" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F197" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="H197" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="198" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F198" t="s">
         <v>207</v>
       </c>
       <c r="H198" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="199" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F199" t="s">
         <v>208</v>
       </c>
       <c r="H199" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="200" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F200" t="s">
         <v>209</v>
       </c>
       <c r="H200" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="201" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F201" t="s">
         <v>215</v>
       </c>
       <c r="H201" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="202" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F202" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="H202" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="203" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F203" t="s">
         <v>225</v>
       </c>
       <c r="H203" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="204" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F204" t="s">
         <v>226</v>
       </c>
       <c r="H204" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="205" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F205" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="H205" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="206" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F206" t="s">
         <v>287</v>
       </c>
       <c r="H206" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="207" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F207" t="s">
         <v>288</v>
       </c>
       <c r="H207" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="208" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F208" t="s">
         <v>289</v>
       </c>
       <c r="H208" t="s">
-        <v>534</v>
+        <v>544</v>
       </c>
     </row>
     <row r="209" spans="6:8" x14ac:dyDescent="0.25">
@@ -5276,7 +4633,7 @@
         <v>290</v>
       </c>
       <c r="H209" t="s">
-        <v>535</v>
+        <v>545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>